<commit_message>
Vendredi 4 juin avance
</commit_message>
<xml_diff>
--- a/lignes.xlsx
+++ b/lignes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IsraelPapuchis\OneDrive\INSA\3TC\2do_semestre\PTIR\PIR-7\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador.000\GitHub\PIR-7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{285FE1BD-517C-4C56-8C10-E05C93AC24A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5BBB13C-D171-47BC-9DAE-55E05992CD4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13800" yWindow="1884" windowWidth="9240" windowHeight="9024" activeTab="1" xr2:uid="{86F50E36-EC87-49B0-9046-7AED0F72F870}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="2" xr2:uid="{86F50E36-EC87-49B0-9046-7AED0F72F870}"/>
   </bookViews>
   <sheets>
     <sheet name="UE" sheetId="1" r:id="rId1"/>
@@ -1009,6 +1009,17 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1027,20 +1038,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1065,7 +1065,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1367,51 +1367,51 @@
       <selection activeCell="U13" sqref="U13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="70.109375" customWidth="1"/>
-    <col min="7" max="7" width="48.88671875" customWidth="1"/>
-    <col min="8" max="8" width="10.109375" customWidth="1"/>
-    <col min="9" max="9" width="10.5546875" customWidth="1"/>
-    <col min="10" max="10" width="42.88671875" customWidth="1"/>
-    <col min="14" max="14" width="47.77734375" customWidth="1"/>
-    <col min="15" max="15" width="14.88671875" customWidth="1"/>
-    <col min="16" max="16" width="16.5546875" customWidth="1"/>
-    <col min="17" max="17" width="40.33203125" customWidth="1"/>
-    <col min="21" max="21" width="48.6640625" customWidth="1"/>
-    <col min="24" max="24" width="39.21875" customWidth="1"/>
+    <col min="2" max="2" width="70.140625" customWidth="1"/>
+    <col min="7" max="7" width="48.85546875" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" customWidth="1"/>
+    <col min="10" max="10" width="42.85546875" customWidth="1"/>
+    <col min="14" max="14" width="47.7109375" customWidth="1"/>
+    <col min="15" max="15" width="14.85546875" customWidth="1"/>
+    <col min="16" max="16" width="16.5703125" customWidth="1"/>
+    <col min="17" max="17" width="40.28515625" customWidth="1"/>
+    <col min="21" max="21" width="48.7109375" customWidth="1"/>
+    <col min="24" max="24" width="39.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A1" s="63" t="s">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A1" s="68" t="s">
         <v>126</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="F1" s="63" t="s">
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="F1" s="68" t="s">
         <v>128</v>
       </c>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
-      <c r="I1" s="64"/>
-      <c r="J1" s="65"/>
-      <c r="M1" s="63" t="s">
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="70"/>
+      <c r="M1" s="68" t="s">
         <v>129</v>
       </c>
-      <c r="N1" s="64"/>
-      <c r="O1" s="64"/>
-      <c r="P1" s="64"/>
-      <c r="Q1" s="65"/>
-      <c r="T1" s="63" t="s">
+      <c r="N1" s="69"/>
+      <c r="O1" s="69"/>
+      <c r="P1" s="69"/>
+      <c r="Q1" s="70"/>
+      <c r="T1" s="68" t="s">
         <v>130</v>
       </c>
-      <c r="U1" s="64"/>
-      <c r="V1" s="64"/>
-      <c r="W1" s="64"/>
-      <c r="X1" s="65"/>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="U1" s="69"/>
+      <c r="V1" s="69"/>
+      <c r="W1" s="69"/>
+      <c r="X1" s="70"/>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>67</v>
       </c>
@@ -1470,7 +1470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="24">
         <v>15</v>
       </c>
@@ -1481,29 +1481,29 @@
         <v>69</v>
       </c>
       <c r="D3" s="26"/>
-      <c r="F3" s="60" t="s">
+      <c r="F3" s="65" t="s">
         <v>113</v>
       </c>
-      <c r="G3" s="61"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="61"/>
-      <c r="J3" s="62"/>
-      <c r="M3" s="60" t="s">
+      <c r="G3" s="66"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="66"/>
+      <c r="J3" s="67"/>
+      <c r="M3" s="65" t="s">
         <v>113</v>
       </c>
-      <c r="N3" s="61"/>
-      <c r="O3" s="61"/>
-      <c r="P3" s="61"/>
-      <c r="Q3" s="62"/>
-      <c r="T3" s="60" t="s">
+      <c r="N3" s="66"/>
+      <c r="O3" s="66"/>
+      <c r="P3" s="66"/>
+      <c r="Q3" s="67"/>
+      <c r="T3" s="65" t="s">
         <v>113</v>
       </c>
-      <c r="U3" s="61"/>
-      <c r="V3" s="61"/>
-      <c r="W3" s="61"/>
-      <c r="X3" s="62"/>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="U3" s="66"/>
+      <c r="V3" s="66"/>
+      <c r="W3" s="66"/>
+      <c r="X3" s="67"/>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="29">
         <v>17</v>
       </c>
@@ -1560,7 +1560,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="33">
         <v>18</v>
       </c>
@@ -1617,7 +1617,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="37">
         <v>19</v>
       </c>
@@ -1674,7 +1674,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="35">
         <v>74</v>
       </c>
@@ -1731,7 +1731,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="37">
         <v>76</v>
       </c>
@@ -1778,7 +1778,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="39">
         <v>84</v>
       </c>
@@ -1787,29 +1787,29 @@
       </c>
       <c r="C9" s="41"/>
       <c r="D9" s="41"/>
-      <c r="F9" s="60" t="s">
+      <c r="F9" s="65" t="s">
         <v>74</v>
       </c>
-      <c r="G9" s="61"/>
-      <c r="H9" s="61"/>
-      <c r="I9" s="61"/>
-      <c r="J9" s="62"/>
-      <c r="M9" s="60" t="s">
+      <c r="G9" s="66"/>
+      <c r="H9" s="66"/>
+      <c r="I9" s="66"/>
+      <c r="J9" s="67"/>
+      <c r="M9" s="65" t="s">
         <v>74</v>
       </c>
-      <c r="N9" s="61"/>
-      <c r="O9" s="61"/>
-      <c r="P9" s="61"/>
-      <c r="Q9" s="62"/>
-      <c r="T9" s="60" t="s">
+      <c r="N9" s="66"/>
+      <c r="O9" s="66"/>
+      <c r="P9" s="66"/>
+      <c r="Q9" s="67"/>
+      <c r="T9" s="65" t="s">
         <v>74</v>
       </c>
-      <c r="U9" s="61"/>
-      <c r="V9" s="61"/>
-      <c r="W9" s="61"/>
-      <c r="X9" s="62"/>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="U9" s="66"/>
+      <c r="V9" s="66"/>
+      <c r="W9" s="66"/>
+      <c r="X9" s="67"/>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="43">
         <v>85</v>
       </c>
@@ -1864,7 +1864,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="43">
         <v>193</v>
       </c>
@@ -1919,7 +1919,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="39">
         <v>194</v>
       </c>
@@ -1928,29 +1928,29 @@
       </c>
       <c r="C12" s="42"/>
       <c r="D12" s="42"/>
-      <c r="F12" s="60" t="s">
+      <c r="F12" s="65" t="s">
         <v>75</v>
       </c>
-      <c r="G12" s="61"/>
-      <c r="H12" s="61"/>
-      <c r="I12" s="61"/>
-      <c r="J12" s="62"/>
-      <c r="M12" s="60" t="s">
+      <c r="G12" s="66"/>
+      <c r="H12" s="66"/>
+      <c r="I12" s="66"/>
+      <c r="J12" s="67"/>
+      <c r="M12" s="65" t="s">
         <v>75</v>
       </c>
-      <c r="N12" s="61"/>
-      <c r="O12" s="61"/>
-      <c r="P12" s="61"/>
-      <c r="Q12" s="62"/>
-      <c r="T12" s="60" t="s">
+      <c r="N12" s="66"/>
+      <c r="O12" s="66"/>
+      <c r="P12" s="66"/>
+      <c r="Q12" s="67"/>
+      <c r="T12" s="65" t="s">
         <v>75</v>
       </c>
-      <c r="U12" s="61"/>
-      <c r="V12" s="61"/>
-      <c r="W12" s="61"/>
-      <c r="X12" s="62"/>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="U12" s="66"/>
+      <c r="V12" s="66"/>
+      <c r="W12" s="66"/>
+      <c r="X12" s="67"/>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="45">
         <v>265</v>
       </c>
@@ -2005,7 +2005,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="48">
         <v>318</v>
       </c>
@@ -2060,7 +2060,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="48">
         <v>321</v>
       </c>
@@ -2115,7 +2115,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="50">
         <v>376</v>
       </c>
@@ -2170,7 +2170,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" s="50">
         <v>384</v>
       </c>
@@ -2225,7 +2225,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" s="55">
         <v>430</v>
       </c>
@@ -2280,7 +2280,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" s="24">
         <v>530</v>
       </c>
@@ -2335,7 +2335,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" s="27">
         <v>542</v>
       </c>
@@ -2390,7 +2390,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" s="39">
         <v>552</v>
       </c>
@@ -2445,7 +2445,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" s="31">
         <v>553</v>
       </c>
@@ -2454,29 +2454,29 @@
       </c>
       <c r="C22" s="32"/>
       <c r="D22" s="2"/>
-      <c r="F22" s="60" t="s">
+      <c r="F22" s="65" t="s">
         <v>115</v>
       </c>
-      <c r="G22" s="61"/>
-      <c r="H22" s="61"/>
-      <c r="I22" s="61"/>
-      <c r="J22" s="62"/>
-      <c r="M22" s="60" t="s">
+      <c r="G22" s="66"/>
+      <c r="H22" s="66"/>
+      <c r="I22" s="66"/>
+      <c r="J22" s="67"/>
+      <c r="M22" s="65" t="s">
         <v>115</v>
       </c>
-      <c r="N22" s="61"/>
-      <c r="O22" s="61"/>
-      <c r="P22" s="61"/>
-      <c r="Q22" s="62"/>
-      <c r="T22" s="60" t="s">
+      <c r="N22" s="66"/>
+      <c r="O22" s="66"/>
+      <c r="P22" s="66"/>
+      <c r="Q22" s="67"/>
+      <c r="T22" s="65" t="s">
         <v>115</v>
       </c>
-      <c r="U22" s="61"/>
-      <c r="V22" s="61"/>
-      <c r="W22" s="61"/>
-      <c r="X22" s="62"/>
-    </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="U22" s="66"/>
+      <c r="V22" s="66"/>
+      <c r="W22" s="66"/>
+      <c r="X22" s="67"/>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" s="27">
         <v>554</v>
       </c>
@@ -2531,7 +2531,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" s="16"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -2582,7 +2582,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="F25" s="16">
         <v>490</v>
       </c>
@@ -2629,7 +2629,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="F26" s="20">
         <v>516</v>
       </c>
@@ -2676,7 +2676,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="F27" s="16">
         <v>523</v>
       </c>
@@ -2723,7 +2723,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="F28" s="16">
         <v>543</v>
       </c>
@@ -2772,6 +2772,8 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="F1:J1"/>
     <mergeCell ref="F22:J22"/>
     <mergeCell ref="T1:X1"/>
     <mergeCell ref="T3:X3"/>
@@ -2786,8 +2788,6 @@
     <mergeCell ref="F3:J3"/>
     <mergeCell ref="F9:J9"/>
     <mergeCell ref="F12:J12"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="F1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2798,26 +2798,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{117DF1EA-6BE1-4C7F-B199-5CE7D0551E2C}">
   <dimension ref="B1:F43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="45.77734375" customWidth="1"/>
-    <col min="6" max="6" width="39.109375" customWidth="1"/>
+    <col min="3" max="3" width="45.7109375" customWidth="1"/>
+    <col min="6" max="6" width="39.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B1" s="63" t="s">
+    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="68" t="s">
         <v>129</v>
       </c>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="65"/>
-    </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="70"/>
+    </row>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="17" t="s">
         <v>67</v>
       </c>
@@ -2834,16 +2834,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B3" s="60" t="s">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="65" t="s">
         <v>113</v>
       </c>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="62"/>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C3" s="66"/>
+      <c r="D3" s="66"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="67"/>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="16">
         <v>12</v>
       </c>
@@ -2860,7 +2860,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="16">
         <v>63</v>
       </c>
@@ -2877,7 +2877,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="16">
         <v>180</v>
       </c>
@@ -2894,7 +2894,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="16">
         <v>184</v>
       </c>
@@ -2911,23 +2911,23 @@
         <v>135</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="16"/>
       <c r="C8" s="3"/>
       <c r="D8" s="16"/>
       <c r="E8" s="16"/>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B9" s="60" t="s">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="65" t="s">
         <v>74</v>
       </c>
-      <c r="C9" s="61"/>
-      <c r="D9" s="61"/>
-      <c r="E9" s="61"/>
-      <c r="F9" s="62"/>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C9" s="66"/>
+      <c r="D9" s="66"/>
+      <c r="E9" s="66"/>
+      <c r="F9" s="67"/>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="16">
         <v>5810</v>
       </c>
@@ -2944,7 +2944,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="16">
         <v>6232</v>
       </c>
@@ -2961,16 +2961,16 @@
         <v>111</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B12" s="60" t="s">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="65" t="s">
         <v>75</v>
       </c>
-      <c r="C12" s="61"/>
-      <c r="D12" s="61"/>
-      <c r="E12" s="61"/>
-      <c r="F12" s="62"/>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C12" s="66"/>
+      <c r="D12" s="66"/>
+      <c r="E12" s="66"/>
+      <c r="F12" s="67"/>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="16">
         <v>8318</v>
       </c>
@@ -2987,120 +2987,120 @@
         <v>114</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B14" s="66">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="60">
         <v>8348</v>
       </c>
       <c r="C14" t="s">
         <v>140</v>
       </c>
-      <c r="D14" s="66" t="s">
-        <v>57</v>
-      </c>
-      <c r="E14" s="66" t="s">
+      <c r="D14" s="60" t="s">
+        <v>57</v>
+      </c>
+      <c r="E14" s="60" t="s">
         <v>86</v>
       </c>
       <c r="F14" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B15" s="66">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="60">
         <v>8354</v>
       </c>
       <c r="C15" t="s">
         <v>134</v>
       </c>
-      <c r="D15" s="66" t="s">
-        <v>86</v>
-      </c>
-      <c r="E15" s="66" t="s">
+      <c r="D15" s="60" t="s">
+        <v>86</v>
+      </c>
+      <c r="E15" s="60" t="s">
         <v>57</v>
       </c>
       <c r="F15" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B16" s="66">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="60">
         <v>8358</v>
       </c>
       <c r="C16" t="s">
         <v>142</v>
       </c>
-      <c r="D16" s="66" t="s">
-        <v>57</v>
-      </c>
-      <c r="E16" s="66" t="s">
+      <c r="D16" s="60" t="s">
+        <v>57</v>
+      </c>
+      <c r="E16" s="60" t="s">
         <v>56</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B17" s="66">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="60">
         <v>8604</v>
       </c>
       <c r="C17" t="s">
         <v>170</v>
       </c>
-      <c r="D17" s="66" t="s">
-        <v>56</v>
-      </c>
-      <c r="E17" s="66" t="s">
+      <c r="D17" s="60" t="s">
+        <v>56</v>
+      </c>
+      <c r="E17" s="60" t="s">
         <v>57</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B18" s="69">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="63">
         <v>8628</v>
       </c>
-      <c r="C18" s="70" t="s">
+      <c r="C18" s="64" t="s">
         <v>172</v>
       </c>
-      <c r="D18" s="70"/>
-      <c r="E18" s="70"/>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B19" s="68">
+      <c r="D18" s="64"/>
+      <c r="E18" s="64"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="62">
         <v>8640</v>
       </c>
       <c r="C19" t="s">
         <v>171</v>
       </c>
-      <c r="D19" s="68" t="s">
-        <v>57</v>
-      </c>
-      <c r="E19" s="68" t="s">
+      <c r="D19" s="62" t="s">
+        <v>57</v>
+      </c>
+      <c r="E19" s="62" t="s">
         <v>56</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B20" s="68">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="62">
         <v>8889</v>
       </c>
       <c r="C20" t="s">
         <v>170</v>
       </c>
-      <c r="D20" s="68" t="s">
-        <v>56</v>
-      </c>
-      <c r="E20" s="68" t="s">
+      <c r="D20" s="62" t="s">
+        <v>56</v>
+      </c>
+      <c r="E20" s="62" t="s">
         <v>57</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B21" s="68">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="62">
         <v>8925</v>
       </c>
       <c r="C21" t="s">
@@ -3116,49 +3116,49 @@
         <v>91</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B22" s="68">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="62">
         <v>9172</v>
       </c>
       <c r="C22" t="s">
         <v>174</v>
       </c>
-      <c r="D22" s="68" t="s">
-        <v>56</v>
-      </c>
-      <c r="E22" s="68" t="s">
+      <c r="D22" s="62" t="s">
+        <v>56</v>
+      </c>
+      <c r="E22" s="62" t="s">
         <v>57</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B23" s="68">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="62">
         <v>9233</v>
       </c>
       <c r="C23" t="s">
         <v>134</v>
       </c>
-      <c r="D23" s="68" t="s">
-        <v>86</v>
-      </c>
-      <c r="E23" s="68" t="s">
+      <c r="D23" s="62" t="s">
+        <v>86</v>
+      </c>
+      <c r="E23" s="62" t="s">
         <v>57</v>
       </c>
       <c r="F23" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B24" s="68">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="62">
         <v>9266</v>
       </c>
       <c r="C24" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" s="16">
         <v>260</v>
       </c>
@@ -3175,7 +3175,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" s="16">
         <v>266</v>
       </c>
@@ -3192,7 +3192,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31" s="16">
         <v>311</v>
       </c>
@@ -3209,7 +3209,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32" s="16">
         <v>322</v>
       </c>
@@ -3226,7 +3226,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33" s="20">
         <v>338</v>
       </c>
@@ -3243,7 +3243,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" s="20">
         <v>355</v>
       </c>
@@ -3260,7 +3260,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35" s="20">
         <v>371</v>
       </c>
@@ -3277,7 +3277,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36" s="20">
         <v>385</v>
       </c>
@@ -3294,7 +3294,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B37" s="21" t="s">
         <v>115</v>
       </c>
@@ -3303,7 +3303,7 @@
       <c r="E37" s="22"/>
       <c r="F37" s="23"/>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B38" s="16">
         <v>429</v>
       </c>
@@ -3320,7 +3320,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B39" s="16">
         <v>441</v>
       </c>
@@ -3337,7 +3337,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B40" s="16">
         <v>490</v>
       </c>
@@ -3354,7 +3354,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B41" s="20">
         <v>516</v>
       </c>
@@ -3371,7 +3371,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B42" s="16">
         <v>523</v>
       </c>
@@ -3388,7 +3388,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B43" s="16">
         <v>543</v>
       </c>
@@ -3420,26 +3420,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C80E785F-0673-4740-B776-36D78552941A}">
   <dimension ref="B1:F28"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="46.5546875" customWidth="1"/>
-    <col min="6" max="6" width="39.88671875" customWidth="1"/>
+    <col min="3" max="3" width="46.5703125" customWidth="1"/>
+    <col min="6" max="6" width="39.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B1" s="63" t="s">
+    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="68" t="s">
         <v>130</v>
       </c>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="65"/>
-    </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="70"/>
+    </row>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="17" t="s">
         <v>67</v>
       </c>
@@ -3456,16 +3456,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B3" s="60" t="s">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="65" t="s">
         <v>113</v>
       </c>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="62"/>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C3" s="66"/>
+      <c r="D3" s="66"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="67"/>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="16">
         <v>26</v>
       </c>
@@ -3482,7 +3482,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="16">
         <v>33</v>
       </c>
@@ -3499,7 +3499,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="16">
         <v>34</v>
       </c>
@@ -3516,24 +3516,24 @@
         <v>148</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B7" s="66">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="60">
         <v>48</v>
       </c>
       <c r="C7" t="s">
         <v>163</v>
       </c>
-      <c r="D7" s="66" t="s">
-        <v>86</v>
-      </c>
-      <c r="E7" s="66" t="s">
+      <c r="D7" s="60" t="s">
+        <v>86</v>
+      </c>
+      <c r="E7" s="60" t="s">
         <v>164</v>
       </c>
-      <c r="F7" s="67" t="s">
+      <c r="F7" s="61" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="16">
         <v>49</v>
       </c>
@@ -3550,42 +3550,42 @@
         <v>150</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B9" s="66">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="60">
         <v>56</v>
       </c>
       <c r="C9" t="s">
         <v>165</v>
       </c>
-      <c r="D9" s="66" t="s">
-        <v>86</v>
-      </c>
-      <c r="E9" s="66" t="s">
+      <c r="D9" s="60" t="s">
+        <v>86</v>
+      </c>
+      <c r="E9" s="60" t="s">
         <v>164</v>
       </c>
       <c r="F9" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="16">
         <v>58</v>
       </c>
       <c r="C10" t="s">
         <v>149</v>
       </c>
-      <c r="D10" s="66" t="s">
+      <c r="D10" s="60" t="s">
         <v>164</v>
       </c>
-      <c r="E10" s="66" t="s">
+      <c r="E10" s="60" t="s">
         <v>86</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B11" s="66">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="60">
         <v>69</v>
       </c>
       <c r="C11" t="s">
@@ -3595,8 +3595,8 @@
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B12" s="66">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="60">
         <v>80</v>
       </c>
       <c r="C12" t="s">
@@ -3608,16 +3608,16 @@
         <v>153</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B13" s="60" t="s">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="65" t="s">
         <v>74</v>
       </c>
-      <c r="C13" s="61"/>
-      <c r="D13" s="61"/>
-      <c r="E13" s="61"/>
-      <c r="F13" s="62"/>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C13" s="66"/>
+      <c r="D13" s="66"/>
+      <c r="E13" s="66"/>
+      <c r="F13" s="67"/>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="16">
         <v>80</v>
       </c>
@@ -3634,7 +3634,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="16">
         <v>88</v>
       </c>
@@ -3651,23 +3651,23 @@
         <v>155</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B16" s="21" t="s">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="65" t="s">
         <v>75</v>
       </c>
-      <c r="C16" s="22"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="23"/>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C16" s="66"/>
+      <c r="D16" s="66"/>
+      <c r="E16" s="66"/>
+      <c r="F16" s="67"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="16"/>
       <c r="C17" s="3"/>
       <c r="D17" s="16"/>
       <c r="E17" s="16"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="16">
         <v>107</v>
       </c>
@@ -3684,7 +3684,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="16">
         <v>109</v>
       </c>
@@ -3701,7 +3701,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="16">
         <v>114</v>
       </c>
@@ -3718,56 +3718,56 @@
         <v>159</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="20"/>
       <c r="C21" s="3"/>
       <c r="D21" s="16"/>
       <c r="E21" s="16"/>
       <c r="F21" s="3"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B22" s="60"/>
-      <c r="C22" s="61"/>
-      <c r="D22" s="61"/>
-      <c r="E22" s="61"/>
-      <c r="F22" s="62"/>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="65"/>
+      <c r="C22" s="66"/>
+      <c r="D22" s="66"/>
+      <c r="E22" s="66"/>
+      <c r="F22" s="67"/>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="16"/>
       <c r="C23" s="3"/>
       <c r="D23" s="16"/>
       <c r="E23" s="16"/>
       <c r="F23" s="19"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="16"/>
       <c r="C24" s="3"/>
       <c r="D24" s="16"/>
       <c r="E24" s="16"/>
       <c r="F24" s="19"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="16"/>
       <c r="C25" s="3"/>
       <c r="D25" s="16"/>
       <c r="E25" s="16"/>
       <c r="F25" s="19"/>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="20"/>
       <c r="C26" s="3"/>
       <c r="D26" s="20"/>
       <c r="E26" s="20"/>
       <c r="F26" s="19"/>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="16"/>
       <c r="C27" s="3"/>
       <c r="D27" s="16"/>
       <c r="E27" s="16"/>
       <c r="F27" s="3"/>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="16"/>
       <c r="C28" s="3"/>
       <c r="D28" s="16"/>
@@ -3775,11 +3775,12 @@
       <c r="F28" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="B13:F13"/>
     <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B16:F16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3793,13 +3794,13 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="40.88671875" customWidth="1"/>
-    <col min="3" max="3" width="132.21875" customWidth="1"/>
+    <col min="2" max="2" width="40.85546875" customWidth="1"/>
+    <col min="3" max="3" width="132.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
@@ -3810,7 +3811,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -3821,7 +3822,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>14</v>
       </c>
@@ -3832,7 +3833,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>18</v>
       </c>
@@ -3843,7 +3844,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
@@ -3854,7 +3855,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>22</v>
       </c>
@@ -3865,7 +3866,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>16</v>
       </c>
@@ -3876,7 +3877,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>24</v>
       </c>
@@ -3887,7 +3888,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>27</v>
       </c>
@@ -3898,7 +3899,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>30</v>
       </c>
@@ -3907,7 +3908,7 @@
       </c>
       <c r="C10" s="3"/>
     </row>
-    <row r="11" spans="1:3" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>32</v>
       </c>
@@ -3918,7 +3919,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>35</v>
       </c>
@@ -3929,7 +3930,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>39</v>
       </c>
@@ -3940,7 +3941,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>41</v>
       </c>
@@ -3949,7 +3950,7 @@
       </c>
       <c r="C14" s="3"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>43</v>
       </c>
@@ -3958,7 +3959,7 @@
       </c>
       <c r="C15" s="3"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
         <v>58</v>
       </c>
@@ -3969,7 +3970,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>61</v>
       </c>
@@ -3980,7 +3981,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
         <v>64</v>
       </c>
@@ -3991,7 +3992,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
         <v>39</v>
       </c>
@@ -4000,7 +4001,7 @@
       </c>
       <c r="C19" s="3"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
         <v>97</v>
       </c>
@@ -4011,7 +4012,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="59" t="s">
         <v>104</v>
       </c>

</xml_diff>

<commit_message>
Avancement mardi 9 juin
</commit_message>
<xml_diff>
--- a/lignes.xlsx
+++ b/lignes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IsraelPapuchis\OneDrive\INSA\3TC\2do_semestre\PTIR\PIR-7\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador.000\GitHub\PIR-7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{629A5BB0-DA6C-464C-9F20-660D5EBFB689}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE85F864-D911-4D2A-838F-7ABF4D7F4548}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{86F50E36-EC87-49B0-9046-7AED0F72F870}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{86F50E36-EC87-49B0-9046-7AED0F72F870}"/>
   </bookViews>
   <sheets>
     <sheet name="UE" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="201">
   <si>
     <t>Description</t>
   </si>
@@ -729,6 +729,9 @@
   </si>
   <si>
     <t>Cell Search</t>
+  </si>
+  <si>
+    <t>Received S1SetupResponse</t>
   </si>
 </sst>
 </file>
@@ -1058,31 +1061,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1093,6 +1072,30 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1104,7 +1107,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1129,7 +1132,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1431,49 +1434,49 @@
       <selection activeCell="F20" sqref="F20:J20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="70.109375" customWidth="1"/>
-    <col min="7" max="7" width="48.88671875" customWidth="1"/>
-    <col min="8" max="8" width="10.109375" customWidth="1"/>
-    <col min="9" max="9" width="10.5546875" customWidth="1"/>
-    <col min="10" max="10" width="42.88671875" customWidth="1"/>
-    <col min="14" max="14" width="47.77734375" customWidth="1"/>
-    <col min="15" max="15" width="14.88671875" customWidth="1"/>
-    <col min="16" max="16" width="16.5546875" customWidth="1"/>
-    <col min="17" max="17" width="40.33203125" customWidth="1"/>
-    <col min="21" max="21" width="48.6640625" customWidth="1"/>
-    <col min="24" max="24" width="39.21875" customWidth="1"/>
+    <col min="2" max="2" width="70.140625" customWidth="1"/>
+    <col min="7" max="7" width="48.85546875" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" customWidth="1"/>
+    <col min="10" max="10" width="42.85546875" customWidth="1"/>
+    <col min="14" max="14" width="47.7109375" customWidth="1"/>
+    <col min="15" max="15" width="14.85546875" customWidth="1"/>
+    <col min="16" max="16" width="16.5703125" customWidth="1"/>
+    <col min="17" max="17" width="40.28515625" customWidth="1"/>
+    <col min="21" max="21" width="48.7109375" customWidth="1"/>
+    <col min="24" max="24" width="39.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A1" s="57" t="s">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A1" s="62" t="s">
         <v>126</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="F1" s="57" t="s">
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="F1" s="62" t="s">
         <v>128</v>
       </c>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="59"/>
-      <c r="M1" s="57" t="s">
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="64"/>
+      <c r="M1" s="62" t="s">
         <v>129</v>
       </c>
-      <c r="N1" s="58"/>
-      <c r="O1" s="58"/>
-      <c r="P1" s="58"/>
-      <c r="Q1" s="59"/>
-      <c r="T1" s="57"/>
-      <c r="U1" s="58"/>
-      <c r="V1" s="58"/>
-      <c r="W1" s="58"/>
-      <c r="X1" s="59"/>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="N1" s="63"/>
+      <c r="O1" s="63"/>
+      <c r="P1" s="63"/>
+      <c r="Q1" s="64"/>
+      <c r="T1" s="62"/>
+      <c r="U1" s="63"/>
+      <c r="V1" s="63"/>
+      <c r="W1" s="63"/>
+      <c r="X1" s="64"/>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>67</v>
       </c>
@@ -1522,7 +1525,7 @@
       <c r="W2" s="17"/>
       <c r="X2" s="17"/>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="21">
         <v>15</v>
       </c>
@@ -1533,27 +1536,27 @@
         <v>69</v>
       </c>
       <c r="D3" s="23"/>
-      <c r="F3" s="60" t="s">
+      <c r="F3" s="65" t="s">
         <v>113</v>
       </c>
-      <c r="G3" s="61"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="61"/>
-      <c r="J3" s="62"/>
-      <c r="M3" s="60" t="s">
+      <c r="G3" s="66"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="66"/>
+      <c r="J3" s="67"/>
+      <c r="M3" s="65" t="s">
         <v>113</v>
       </c>
-      <c r="N3" s="61"/>
-      <c r="O3" s="61"/>
-      <c r="P3" s="61"/>
-      <c r="Q3" s="62"/>
-      <c r="T3" s="60"/>
-      <c r="U3" s="61"/>
-      <c r="V3" s="61"/>
-      <c r="W3" s="61"/>
-      <c r="X3" s="62"/>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="N3" s="66"/>
+      <c r="O3" s="66"/>
+      <c r="P3" s="66"/>
+      <c r="Q3" s="67"/>
+      <c r="T3" s="65"/>
+      <c r="U3" s="66"/>
+      <c r="V3" s="66"/>
+      <c r="W3" s="66"/>
+      <c r="X3" s="67"/>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="26">
         <v>17</v>
       </c>
@@ -1600,7 +1603,7 @@
       <c r="W4" s="20"/>
       <c r="X4" s="19"/>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="30">
         <v>18</v>
       </c>
@@ -1647,7 +1650,7 @@
       <c r="W5" s="20"/>
       <c r="X5" s="19"/>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="34">
         <v>19</v>
       </c>
@@ -1694,7 +1697,7 @@
       <c r="W6" s="20"/>
       <c r="X6" s="19"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="32">
         <v>74</v>
       </c>
@@ -1741,7 +1744,7 @@
       <c r="W7" s="16"/>
       <c r="X7" s="3"/>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="34">
         <v>76</v>
       </c>
@@ -1778,7 +1781,7 @@
       <c r="W8" s="16"/>
       <c r="X8" s="3"/>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="36">
         <v>84</v>
       </c>
@@ -1787,27 +1790,27 @@
       </c>
       <c r="C9" s="38"/>
       <c r="D9" s="38"/>
-      <c r="F9" s="60" t="s">
+      <c r="F9" s="65" t="s">
         <v>74</v>
       </c>
-      <c r="G9" s="61"/>
-      <c r="H9" s="61"/>
-      <c r="I9" s="61"/>
-      <c r="J9" s="62"/>
-      <c r="M9" s="60" t="s">
+      <c r="G9" s="66"/>
+      <c r="H9" s="66"/>
+      <c r="I9" s="66"/>
+      <c r="J9" s="67"/>
+      <c r="M9" s="65" t="s">
         <v>74</v>
       </c>
-      <c r="N9" s="61"/>
-      <c r="O9" s="61"/>
-      <c r="P9" s="61"/>
-      <c r="Q9" s="62"/>
-      <c r="T9" s="60"/>
-      <c r="U9" s="61"/>
-      <c r="V9" s="61"/>
-      <c r="W9" s="61"/>
-      <c r="X9" s="62"/>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="N9" s="66"/>
+      <c r="O9" s="66"/>
+      <c r="P9" s="66"/>
+      <c r="Q9" s="67"/>
+      <c r="T9" s="65"/>
+      <c r="U9" s="66"/>
+      <c r="V9" s="66"/>
+      <c r="W9" s="66"/>
+      <c r="X9" s="67"/>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="40">
         <v>85</v>
       </c>
@@ -1852,7 +1855,7 @@
       <c r="W10" s="20"/>
       <c r="X10" s="19"/>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="40">
         <v>193</v>
       </c>
@@ -1897,7 +1900,7 @@
       <c r="W11" s="16"/>
       <c r="X11" s="19"/>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="36">
         <v>194</v>
       </c>
@@ -1906,27 +1909,27 @@
       </c>
       <c r="C12" s="39"/>
       <c r="D12" s="39"/>
-      <c r="F12" s="60" t="s">
+      <c r="F12" s="65" t="s">
         <v>75</v>
       </c>
-      <c r="G12" s="61"/>
-      <c r="H12" s="61"/>
-      <c r="I12" s="61"/>
-      <c r="J12" s="62"/>
-      <c r="M12" s="60" t="s">
+      <c r="G12" s="66"/>
+      <c r="H12" s="66"/>
+      <c r="I12" s="66"/>
+      <c r="J12" s="67"/>
+      <c r="M12" s="65" t="s">
         <v>75</v>
       </c>
-      <c r="N12" s="61"/>
-      <c r="O12" s="61"/>
-      <c r="P12" s="61"/>
-      <c r="Q12" s="62"/>
-      <c r="T12" s="60"/>
-      <c r="U12" s="61"/>
-      <c r="V12" s="61"/>
-      <c r="W12" s="61"/>
-      <c r="X12" s="62"/>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="N12" s="66"/>
+      <c r="O12" s="66"/>
+      <c r="P12" s="66"/>
+      <c r="Q12" s="67"/>
+      <c r="T12" s="65"/>
+      <c r="U12" s="66"/>
+      <c r="V12" s="66"/>
+      <c r="W12" s="66"/>
+      <c r="X12" s="67"/>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="42">
         <v>265</v>
       </c>
@@ -1971,7 +1974,7 @@
       <c r="W13" s="16"/>
       <c r="X13" s="3"/>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="45">
         <v>318</v>
       </c>
@@ -2016,7 +2019,7 @@
       <c r="W14" s="16"/>
       <c r="X14" s="3"/>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="45">
         <v>321</v>
       </c>
@@ -2061,7 +2064,7 @@
       <c r="W15" s="16"/>
       <c r="X15" s="3"/>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="47">
         <v>376</v>
       </c>
@@ -2106,7 +2109,7 @@
       <c r="W16" s="16"/>
       <c r="X16" s="3"/>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" s="47">
         <v>384</v>
       </c>
@@ -2151,7 +2154,7 @@
       <c r="W17" s="16"/>
       <c r="X17" s="3"/>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" s="52">
         <v>430</v>
       </c>
@@ -2196,7 +2199,7 @@
       <c r="W18" s="16"/>
       <c r="X18" s="3"/>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" s="21">
         <v>530</v>
       </c>
@@ -2241,7 +2244,7 @@
       <c r="W19" s="16"/>
       <c r="X19" s="3"/>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" s="24">
         <v>542</v>
       </c>
@@ -2250,13 +2253,13 @@
       </c>
       <c r="C20" s="25"/>
       <c r="D20" s="23"/>
-      <c r="F20" s="60" t="s">
+      <c r="F20" s="65" t="s">
         <v>115</v>
       </c>
-      <c r="G20" s="61"/>
-      <c r="H20" s="61"/>
-      <c r="I20" s="61"/>
-      <c r="J20" s="62"/>
+      <c r="G20" s="66"/>
+      <c r="H20" s="66"/>
+      <c r="I20" s="66"/>
+      <c r="J20" s="67"/>
       <c r="M20" s="20">
         <v>371</v>
       </c>
@@ -2278,7 +2281,7 @@
       <c r="W20" s="16"/>
       <c r="X20" s="3"/>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" s="36">
         <v>552</v>
       </c>
@@ -2323,7 +2326,7 @@
       <c r="W21" s="16"/>
       <c r="X21" s="3"/>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" s="28">
         <v>553</v>
       </c>
@@ -2347,20 +2350,20 @@
       <c r="J22" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="M22" s="60" t="s">
+      <c r="M22" s="65" t="s">
         <v>115</v>
       </c>
-      <c r="N22" s="61"/>
-      <c r="O22" s="61"/>
-      <c r="P22" s="61"/>
-      <c r="Q22" s="62"/>
-      <c r="T22" s="60"/>
-      <c r="U22" s="61"/>
-      <c r="V22" s="61"/>
-      <c r="W22" s="61"/>
-      <c r="X22" s="62"/>
-    </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="N22" s="66"/>
+      <c r="O22" s="66"/>
+      <c r="P22" s="66"/>
+      <c r="Q22" s="67"/>
+      <c r="T22" s="65"/>
+      <c r="U22" s="66"/>
+      <c r="V22" s="66"/>
+      <c r="W22" s="66"/>
+      <c r="X22" s="67"/>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" s="24">
         <v>554</v>
       </c>
@@ -2405,7 +2408,7 @@
       <c r="W23" s="16"/>
       <c r="X23" s="19"/>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" s="16"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -2446,7 +2449,7 @@
       <c r="W24" s="16"/>
       <c r="X24" s="19"/>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="F25" s="16">
         <v>523</v>
       </c>
@@ -2483,7 +2486,7 @@
       <c r="W25" s="16"/>
       <c r="X25" s="19"/>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="F26" s="16">
         <v>543</v>
       </c>
@@ -2520,7 +2523,7 @@
       <c r="W26" s="20"/>
       <c r="X26" s="19"/>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="F27" s="20">
         <v>673</v>
       </c>
@@ -2557,7 +2560,7 @@
       <c r="W27" s="16"/>
       <c r="X27" s="3"/>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="M28" s="16">
         <v>543</v>
       </c>
@@ -2579,16 +2582,16 @@
       <c r="W28" s="20"/>
       <c r="X28" s="3"/>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="F29" s="69" t="s">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="F29" s="61" t="s">
         <v>196</v>
       </c>
-      <c r="G29" s="69"/>
-      <c r="H29" s="69"/>
-      <c r="I29" s="69"/>
-      <c r="J29" s="69"/>
-    </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="G29" s="61"/>
+      <c r="H29" s="61"/>
+      <c r="I29" s="61"/>
+      <c r="J29" s="61"/>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="F30" s="20">
         <v>866</v>
       </c>
@@ -2607,6 +2610,7 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="F12:J12"/>
     <mergeCell ref="F29:J29"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="F1:J1"/>
@@ -2623,7 +2627,6 @@
     <mergeCell ref="M22:Q22"/>
     <mergeCell ref="F3:J3"/>
     <mergeCell ref="F9:J9"/>
-    <mergeCell ref="F12:J12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2634,26 +2637,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{117DF1EA-6BE1-4C7F-B199-5CE7D0551E2C}">
   <dimension ref="B1:F38"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="51.6640625" customWidth="1"/>
-    <col min="6" max="6" width="44.77734375" customWidth="1"/>
+    <col min="3" max="3" width="51.7109375" customWidth="1"/>
+    <col min="6" max="6" width="44.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B1" s="57" t="s">
+    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="62" t="s">
         <v>129</v>
       </c>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="59"/>
-    </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="64"/>
+    </row>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="17" t="s">
         <v>67</v>
       </c>
@@ -2670,16 +2673,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B3" s="63" t="s">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="68" t="s">
         <v>113</v>
       </c>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="68"/>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="16">
         <v>12</v>
       </c>
@@ -2696,7 +2699,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="16">
         <v>63</v>
       </c>
@@ -2713,7 +2716,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="16">
         <v>180</v>
       </c>
@@ -2730,12 +2733,12 @@
         <v>154</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="16">
         <v>184</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>134</v>
+        <v>200</v>
       </c>
       <c r="D7" s="16" t="s">
         <v>86</v>
@@ -2747,16 +2750,16 @@
         <v>135</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B8" s="60" t="s">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="65" t="s">
         <v>74</v>
       </c>
-      <c r="C8" s="61"/>
-      <c r="D8" s="61"/>
-      <c r="E8" s="61"/>
-      <c r="F8" s="62"/>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C8" s="66"/>
+      <c r="D8" s="66"/>
+      <c r="E8" s="66"/>
+      <c r="F8" s="67"/>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="16">
         <v>5812</v>
       </c>
@@ -2773,7 +2776,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="16">
         <v>6232</v>
       </c>
@@ -2790,7 +2793,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="16">
         <v>8318</v>
       </c>
@@ -2807,16 +2810,16 @@
         <v>114</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B12" s="63" t="s">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="68" t="s">
         <v>182</v>
       </c>
-      <c r="C12" s="63"/>
-      <c r="D12" s="63"/>
-      <c r="E12" s="63"/>
-      <c r="F12" s="63"/>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C12" s="68"/>
+      <c r="D12" s="68"/>
+      <c r="E12" s="68"/>
+      <c r="F12" s="68"/>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="20">
         <v>8348</v>
       </c>
@@ -2833,7 +2836,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="20">
         <v>8354</v>
       </c>
@@ -2850,7 +2853,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="20">
         <v>8358</v>
       </c>
@@ -2867,7 +2870,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="20">
         <v>8604</v>
       </c>
@@ -2884,7 +2887,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="20">
         <v>8630</v>
       </c>
@@ -2901,7 +2904,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="20">
         <v>8639</v>
       </c>
@@ -2918,7 +2921,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="20">
         <v>8640</v>
       </c>
@@ -2935,7 +2938,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="20">
         <v>8889</v>
       </c>
@@ -2952,7 +2955,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="20">
         <v>8918</v>
       </c>
@@ -2969,7 +2972,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="20">
         <v>8924</v>
       </c>
@@ -2986,7 +2989,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="20">
         <v>8925</v>
       </c>
@@ -3003,7 +3006,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="20">
         <v>9172</v>
       </c>
@@ -3020,16 +3023,16 @@
         <v>92</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B25" s="60" t="s">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="65" t="s">
         <v>115</v>
       </c>
-      <c r="C25" s="61"/>
-      <c r="D25" s="61"/>
-      <c r="E25" s="61"/>
-      <c r="F25" s="62"/>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C25" s="66"/>
+      <c r="D25" s="66"/>
+      <c r="E25" s="66"/>
+      <c r="F25" s="67"/>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="20">
         <v>9236</v>
       </c>
@@ -3046,7 +3049,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="20">
         <v>9266</v>
       </c>
@@ -3063,7 +3066,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="20">
         <v>9503</v>
       </c>
@@ -3080,7 +3083,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" s="20">
         <v>9524</v>
       </c>
@@ -3097,7 +3100,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" s="20">
         <v>9570</v>
       </c>
@@ -3114,7 +3117,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31" s="20">
         <v>10004</v>
       </c>
@@ -3131,7 +3134,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32" s="20">
         <v>10058</v>
       </c>
@@ -3148,33 +3151,33 @@
         <v>90</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B33" s="64" t="s">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" s="57" t="s">
         <v>197</v>
       </c>
-      <c r="C33" s="64"/>
-      <c r="D33" s="64"/>
-      <c r="E33" s="64"/>
-      <c r="F33" s="64"/>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B34" s="68">
+      <c r="C33" s="57"/>
+      <c r="D33" s="57"/>
+      <c r="E33" s="57"/>
+      <c r="F33" s="57"/>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B34" s="60">
         <v>11226</v>
       </c>
-      <c r="C34" s="66" t="s">
+      <c r="C34" s="58" t="s">
         <v>134</v>
       </c>
-      <c r="D34" s="67" t="s">
-        <v>86</v>
-      </c>
-      <c r="E34" s="67" t="s">
-        <v>57</v>
-      </c>
-      <c r="F34" s="66" t="s">
+      <c r="D34" s="59" t="s">
+        <v>86</v>
+      </c>
+      <c r="E34" s="59" t="s">
+        <v>57</v>
+      </c>
+      <c r="F34" s="58" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35" s="20">
         <v>11230</v>
       </c>
@@ -3187,20 +3190,20 @@
       <c r="E35" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="F35" s="66" t="s">
+      <c r="F35" s="58" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B37" s="69" t="s">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B37" s="61" t="s">
         <v>196</v>
       </c>
-      <c r="C37" s="69"/>
-      <c r="D37" s="69"/>
-      <c r="E37" s="69"/>
-      <c r="F37" s="69"/>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C37" s="61"/>
+      <c r="D37" s="61"/>
+      <c r="E37" s="61"/>
+      <c r="F37" s="61"/>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B38" s="20">
         <v>21255</v>
       </c>
@@ -3234,26 +3237,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C80E785F-0673-4740-B776-36D78552941A}">
   <dimension ref="B1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="B22" sqref="B22:F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="46.5546875" customWidth="1"/>
-    <col min="6" max="6" width="39.88671875" customWidth="1"/>
+    <col min="3" max="3" width="46.5703125" customWidth="1"/>
+    <col min="6" max="6" width="39.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B1" s="65" t="s">
+    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="69" t="s">
         <v>130</v>
       </c>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-    </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+    </row>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="17" t="s">
         <v>67</v>
       </c>
@@ -3270,7 +3273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="70" t="s">
         <v>199</v>
       </c>
@@ -3279,7 +3282,7 @@
       <c r="E3" s="71"/>
       <c r="F3" s="72"/>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="16">
         <v>28</v>
       </c>
@@ -3296,7 +3299,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="16">
         <v>33</v>
       </c>
@@ -3313,16 +3316,16 @@
         <v>145</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B6" s="63" t="s">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="68" t="s">
         <v>182</v>
       </c>
-      <c r="C6" s="63"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="63"/>
-      <c r="F6" s="63"/>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C6" s="68"/>
+      <c r="D6" s="68"/>
+      <c r="E6" s="68"/>
+      <c r="F6" s="68"/>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="16">
         <v>36</v>
       </c>
@@ -3339,7 +3342,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="20">
         <v>48</v>
       </c>
@@ -3356,7 +3359,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="16">
         <v>53</v>
       </c>
@@ -3373,7 +3376,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="20">
         <v>56</v>
       </c>
@@ -3390,7 +3393,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="16">
         <v>62</v>
       </c>
@@ -3407,7 +3410,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="20">
         <v>69</v>
       </c>
@@ -3424,7 +3427,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="20">
         <v>85</v>
       </c>
@@ -3441,16 +3444,16 @@
         <v>149</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B14" s="63" t="s">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="68" t="s">
         <v>115</v>
       </c>
-      <c r="C14" s="63"/>
-      <c r="D14" s="63"/>
-      <c r="E14" s="63"/>
-      <c r="F14" s="63"/>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C14" s="68"/>
+      <c r="D14" s="68"/>
+      <c r="E14" s="68"/>
+      <c r="F14" s="68"/>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="16">
         <v>88</v>
       </c>
@@ -3467,7 +3470,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="16">
         <v>107</v>
       </c>
@@ -3484,7 +3487,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="16">
         <v>111</v>
       </c>
@@ -3501,7 +3504,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="16">
         <v>119</v>
       </c>
@@ -3518,7 +3521,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="20">
         <v>136</v>
       </c>
@@ -3535,16 +3538,16 @@
         <v>198</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B22" s="63" t="s">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="68" t="s">
         <v>196</v>
       </c>
-      <c r="C22" s="63"/>
-      <c r="D22" s="63"/>
-      <c r="E22" s="63"/>
-      <c r="F22" s="63"/>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C22" s="68"/>
+      <c r="D22" s="68"/>
+      <c r="E22" s="68"/>
+      <c r="F22" s="68"/>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="20">
         <v>150</v>
       </c>
@@ -3581,13 +3584,13 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="40.88671875" customWidth="1"/>
-    <col min="3" max="3" width="132.21875" customWidth="1"/>
+    <col min="2" max="2" width="40.85546875" customWidth="1"/>
+    <col min="3" max="3" width="132.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
@@ -3598,7 +3601,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -3609,7 +3612,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>14</v>
       </c>
@@ -3620,7 +3623,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>18</v>
       </c>
@@ -3631,7 +3634,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
@@ -3642,7 +3645,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>22</v>
       </c>
@@ -3653,7 +3656,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>16</v>
       </c>
@@ -3664,7 +3667,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>24</v>
       </c>
@@ -3675,7 +3678,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>27</v>
       </c>
@@ -3686,7 +3689,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>30</v>
       </c>
@@ -3695,7 +3698,7 @@
       </c>
       <c r="C10" s="3"/>
     </row>
-    <row r="11" spans="1:3" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>32</v>
       </c>
@@ -3706,7 +3709,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>35</v>
       </c>
@@ -3717,7 +3720,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>39</v>
       </c>
@@ -3728,7 +3731,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>41</v>
       </c>
@@ -3737,7 +3740,7 @@
       </c>
       <c r="C14" s="3"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>43</v>
       </c>
@@ -3746,7 +3749,7 @@
       </c>
       <c r="C15" s="3"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
         <v>58</v>
       </c>
@@ -3757,7 +3760,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>61</v>
       </c>
@@ -3768,7 +3771,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
         <v>64</v>
       </c>
@@ -3779,7 +3782,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
         <v>39</v>
       </c>
@@ -3788,7 +3791,7 @@
       </c>
       <c r="C19" s="3"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
         <v>97</v>
       </c>
@@ -3799,7 +3802,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="56" t="s">
         <v>104</v>
       </c>

</xml_diff>